<commit_message>
cambio a total return
</commit_message>
<xml_diff>
--- a/Crisis/tickers.xlsx
+++ b/Crisis/tickers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\Assorted-Backtests\Crisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966859ED-57C7-4143-80A4-141CE5B36E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A871C28-D2DE-452C-B144-CBFDB7468299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8BDE6E73-C58F-4B49-8B6C-097DC0A7ECE2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="36">
   <si>
     <t>ticker</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>Asia Pacific</t>
+  </si>
+  <si>
+    <t>TOT_RETURN_INDEX_GROSS_DVDS</t>
+  </si>
+  <si>
+    <t>MXFEJ Index</t>
+  </si>
+  <si>
+    <t>Far East ex Japon</t>
   </si>
 </sst>
 </file>
@@ -487,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF93CD93-5A4A-4E2B-88BD-45F485E0AE9A}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +528,7 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -530,7 +539,7 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -541,7 +550,7 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -552,7 +561,7 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -563,7 +572,7 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -574,7 +583,7 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -585,7 +594,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -596,7 +605,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -695,7 +704,7 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -750,7 +759,7 @@
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -772,7 +781,7 @@
         <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -783,6 +792,28 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dictioanry to change fields
</commit_message>
<xml_diff>
--- a/Crisis/tickers.xlsx
+++ b/Crisis/tickers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\Assorted-Backtests\Crisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0524ADA1-913A-4EF1-ACF8-5BA910F7AE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D60A0E-6B77-4DD9-A18B-2300CAD00CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8BDE6E73-C58F-4B49-8B6C-097DC0A7ECE2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="41">
   <si>
     <t>ticker</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>MXWD Index</t>
+  </si>
+  <si>
+    <t>field_short_name</t>
+  </si>
+  <si>
+    <t>Price TR</t>
+  </si>
+  <si>
+    <t>PB Ratio</t>
   </si>
 </sst>
 </file>
@@ -502,20 +511,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF93CD93-5A4A-4E2B-88BD-45F485E0AE9A}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -525,8 +535,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -536,8 +549,11 @@
       <c r="C2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -547,8 +563,11 @@
       <c r="C3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -558,8 +577,11 @@
       <c r="C4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -569,8 +591,11 @@
       <c r="C5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -580,8 +605,11 @@
       <c r="C6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -591,8 +619,11 @@
       <c r="C7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -602,8 +633,11 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -613,8 +647,11 @@
       <c r="C9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -624,8 +661,11 @@
       <c r="C10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -635,8 +675,11 @@
       <c r="C11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -646,8 +689,11 @@
       <c r="C12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -657,8 +703,11 @@
       <c r="C13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -668,8 +717,11 @@
       <c r="C14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -679,8 +731,11 @@
       <c r="C15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -690,8 +745,11 @@
       <c r="C16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -701,8 +759,11 @@
       <c r="C17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -712,8 +773,11 @@
       <c r="C18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -723,8 +787,11 @@
       <c r="C19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -734,8 +801,11 @@
       <c r="C20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -745,8 +815,11 @@
       <c r="C21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -756,8 +829,11 @@
       <c r="C22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -767,8 +843,11 @@
       <c r="C23" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -778,8 +857,11 @@
       <c r="C24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -789,8 +871,11 @@
       <c r="C25" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -800,8 +885,11 @@
       <c r="C26" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -811,8 +899,11 @@
       <c r="C27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -822,8 +913,11 @@
       <c r="C28" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -832,6 +926,9 @@
       </c>
       <c r="C29" t="s">
         <v>36</v>
+      </c>
+      <c r="D29" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>